<commit_message>
Automatische test-sync: 2025-08-04 19:59:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,8 +735,60 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Opvolging / Status</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We hebben je eerdere e-mail ontvangen en doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-04 19:59:12</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -756,7 +808,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -764,17 +816,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,7 +868,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,8 +787,60 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #2: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Opvolging / Status</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We hebben je eerdere e-mail ontvangen en doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:01:22</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -808,7 +860,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,17 +868,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -868,7 +920,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,8 +839,60 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #3: Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We hebben je eerdere e-mail ontvangen en doorgestuurd naar retour@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:03:35</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -860,7 +912,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -868,17 +920,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -893,7 +945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -923,6 +975,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:07:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -891,8 +891,68 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om uw vraag te kunnen beantwoorden, heb ik wat meer informatie nodig. Kunt u mij de volgende gegevens bezorgen:
+1. Het ordernummer van uw aankoop.
+2. De datum waarop de terugbetaling is aangevraagd.
+3. Eventuele referentienummers of andere relevante details.
+Met deze gegevens kan ik uw zaak verder onderzoeken en u van passende ondersteuning voorzien.
+Met vriendelijke groet,
+[Naam] 
+Klantenservice Team</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:07:30</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -912,7 +972,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -920,17 +980,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -982,7 +1042,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1003,8 +1003,60 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:11:50</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1024,7 +1076,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1032,17 +1084,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1104,7 +1156,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:14:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1055,8 +1055,60 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:14:02</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1076,7 +1128,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1084,17 +1136,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1142,17 +1194,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1107,8 +1107,60 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:16:21</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1128,7 +1180,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1136,17 +1188,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1161,7 +1213,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1211,6 +1263,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1215,8 +1215,60 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:20:43</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1236,7 +1288,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1244,17 +1296,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1326,7 +1378,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1267,8 +1267,60 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:26:35</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1288,7 +1340,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1296,17 +1348,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1344,17 +1396,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Opvolging / Status</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Opvolging / Status</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1319,8 +1319,60 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:28:53</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1340,7 +1392,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1348,17 +1400,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1400,7 +1452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1371,8 +1371,60 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:31:25</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1392,7 +1444,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1400,17 +1452,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1452,7 +1504,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:34:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1423,8 +1423,60 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:33:58</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1444,7 +1496,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1452,17 +1504,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1520,17 +1572,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1530,8 +1530,60 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:38:25</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1551,7 +1603,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1559,17 +1611,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1617,17 +1669,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Opvolging / Status</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Opvolging / Status</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1582,8 +1582,60 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:40:33</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1603,7 +1655,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1611,17 +1663,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1673,7 +1725,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1634,8 +1634,60 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:42:45</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1655,7 +1707,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1663,17 +1715,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1725,7 +1777,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1686,8 +1686,60 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Opvolging / Status</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We hebben je eerdere e-mail ontvangen en doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:44:55</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1707,7 +1759,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1715,17 +1767,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1787,7 +1839,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1738,8 +1738,60 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testmail #10: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Opvolging / Status</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We hebben je eerdere e-mail ontvangen en doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:47:04</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1759,7 +1811,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1767,17 +1819,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1839,7 +1891,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:53:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1902,8 +1902,60 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar documentatie@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:53:41</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1923,7 +1975,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1931,17 +1983,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J24">
+  <conditionalFormatting sqref="J2:J25">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1956,7 +2008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1979,7 +2031,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1989,7 +2041,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2024,6 +2076,16 @@
       </c>
       <c r="B6" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1954,8 +1954,60 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar kwaliteit@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:55:52</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1975,7 +2027,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1983,17 +2035,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J25">
+  <conditionalFormatting sqref="J2:J26">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2008,7 +2060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2031,7 +2083,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -2041,7 +2093,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2085,6 +2137,16 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 20:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2006,8 +2006,60 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Testmail #15: Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-08-04 20:58:04</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2027,7 +2079,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2035,17 +2087,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26">
+  <conditionalFormatting sqref="J2:J27">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2087,7 +2139,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 21:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2058,8 +2058,60 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-08-04 21:00:14</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2079,7 +2131,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2087,17 +2139,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J27">
+  <conditionalFormatting sqref="J2:J28">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2139,7 +2191,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 21:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2110,8 +2110,60 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-08-04 21:02:31</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2131,7 +2183,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2139,17 +2191,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J28">
+  <conditionalFormatting sqref="J2:J29">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2191,7 +2243,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-04 21:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-04.xlsx
+++ b/logs/mail_log_2025-08-04.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2162,8 +2162,60 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-08-04 21:04:43</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2183,7 +2235,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2191,17 +2243,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J29">
+  <conditionalFormatting sqref="J2:J30">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2253,7 +2305,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">

</xml_diff>